<commit_message>
BREAKING CHANGE: Added the svm alghorithm functionalities
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -17,13 +17,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <sz val="8"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +52,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,124 +439,205 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:K4"/>
+  <dimension ref="B6:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+  </cols>
   <sheetData>
-    <row r="2">
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Settled Reports Of Violators</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Violator_id</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Enforcer_id</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Extracted_id</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Ticket Number</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Violation</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Barangay</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Plate Number</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Vehicle</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>106</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>TCT-00002</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>speeding, running-red-light, illegal-parking</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1:14 PM</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>06/02/2024</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Santo Domingo</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Republika ng Pilipinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Lungsod ng Santa Rosa</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Lalawigan ng Laguna</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>SANGAY NG PAMAMAHALA AT PAGPAPATUPAD NG TRAPIKO</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>(CITY TRAFFIC MANAGEMENT AND ENFORCEMENT UNIT)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>TRAFFIC CITATION TICKET NO.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>NAME OF APPREHENDED DRIVER/OPERATOR</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>VIOLATION(S)</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>PLACE OF APPREHENSION</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>DRIVER'S LICENSE NO.</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>MV PLATE NO.</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>MUN. PLATE NO.</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>DATE/TIME OF APPREHENSION</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>RECEIVED BY (NAME AND SIGNATURE)</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>RECEIVED DATE</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="4" t="n">
+        <v>131</v>
+      </c>
+      <c r="C13" s="4" t="n"/>
+      <c r="D13" s="4" t="n"/>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>TCT-00028</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>running-red-light, illegal-parking, reckless-driving</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>10:32 AM</t>
+        </is>
+      </c>
+      <c r="H13" s="4" t="inlineStr">
+        <is>
+          <t>06/16/2024</t>
+        </is>
+      </c>
+      <c r="I13" s="4" t="inlineStr">
+        <is>
+          <t>Macabling</t>
+        </is>
+      </c>
+      <c r="J13" s="4" t="inlineStr">
         <is>
           <t>NFW4100</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Jeep</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>settled</t>
+      <c r="K13" s="4" t="inlineStr">
+        <is>
+          <t>Motorcycle</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="4" t="n">
+        <v>109</v>
+      </c>
+      <c r="C14" s="4" t="n"/>
+      <c r="D14" s="4" t="n"/>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>TCT-00005</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>speeding, running-red-light, illegal-parking, reckless-driving, driving-under-influence, failure-to-yield</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>11:19 AM</t>
+        </is>
+      </c>
+      <c r="H14" s="4" t="inlineStr">
+        <is>
+          <t>06/11/2024</t>
+        </is>
+      </c>
+      <c r="I14" s="4" t="inlineStr">
+        <is>
+          <t>Poblacion</t>
+        </is>
+      </c>
+      <c r="J14" s="4" t="inlineStr">
+        <is>
+          <t>NFW4100</t>
+        </is>
+      </c>
+      <c r="K14" s="4" t="inlineStr">
+        <is>
+          <t>Tricycle</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B10:K10"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>